<commit_message>
Updating rnasep2 IFB-Core assembly & annotation pipeline.
</commit_message>
<xml_diff>
--- a/Bioinformatics/Samples_RNAsep1.xlsx
+++ b/Bioinformatics/Samples_RNAsep1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A6DBFE-C20F-6A41-9F4F-603F918319E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D81428-7B33-574A-9B0B-EFF23F961A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1315,10 +1315,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:E6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1356,7 +1357,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="35" t="s">
         <v>37</v>
       </c>
@@ -1369,7 +1370,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="36" t="s">
         <v>40</v>
       </c>
@@ -1377,7 +1378,7 @@
       <c r="E7" s="36"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>193</v>
       </c>
@@ -1464,7 +1465,7 @@
       </c>
       <c r="J10" s="20"/>
     </row>
-    <row r="11" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>148</v>
       </c>
@@ -1517,7 +1518,7 @@
       </c>
       <c r="M12" s="30"/>
     </row>
-    <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>140</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>238688611</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>139</v>
       </c>
@@ -1617,7 +1618,7 @@
       </c>
       <c r="J16" s="20"/>
     </row>
-    <row r="17" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>142</v>
       </c>
@@ -1669,7 +1670,7 @@
       </c>
       <c r="J18" s="20"/>
     </row>
-    <row r="19" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>143</v>
       </c>
@@ -1719,7 +1720,7 @@
       </c>
       <c r="J20" s="20"/>
     </row>
-    <row r="21" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>141</v>
       </c>
@@ -1767,7 +1768,7 @@
       </c>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>150</v>
       </c>
@@ -1819,7 +1820,7 @@
       </c>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>151</v>
       </c>
@@ -1867,7 +1868,7 @@
       </c>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>149</v>
       </c>
@@ -1945,7 +1946,7 @@
       </c>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>154</v>
       </c>
@@ -1963,7 +1964,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>129</v>
       </c>
@@ -1976,11 +1977,11 @@
       <c r="I31" s="5"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I32" s="5"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C33" s="37" t="s">
         <v>41</v>
       </c>
@@ -1989,7 +1990,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>193</v>
       </c>
@@ -2038,7 +2039,7 @@
       </c>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>175</v>
       </c>
@@ -2090,7 +2091,7 @@
       </c>
       <c r="J37" s="20"/>
     </row>
-    <row r="38" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>174</v>
       </c>
@@ -2142,7 +2143,7 @@
       </c>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>176</v>
       </c>
@@ -2194,7 +2195,7 @@
       </c>
       <c r="J41" s="20"/>
     </row>
-    <row r="42" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>179</v>
       </c>
@@ -2242,7 +2243,7 @@
       </c>
       <c r="J43" s="20"/>
     </row>
-    <row r="44" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>180</v>
       </c>
@@ -2294,7 +2295,7 @@
       </c>
       <c r="J45" s="20"/>
     </row>
-    <row r="46" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>182</v>
       </c>
@@ -2346,7 +2347,7 @@
       </c>
       <c r="J47" s="20"/>
     </row>
-    <row r="48" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>185</v>
       </c>
@@ -2394,7 +2395,7 @@
       </c>
       <c r="J49" s="20"/>
     </row>
-    <row r="50" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>184</v>
       </c>
@@ -2472,7 +2473,7 @@
       </c>
       <c r="J52" s="20"/>
     </row>
-    <row r="53" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>188</v>
       </c>
@@ -2524,7 +2525,7 @@
       </c>
       <c r="J54" s="6"/>
     </row>
-    <row r="55" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>189</v>
       </c>
@@ -2572,7 +2573,7 @@
       </c>
       <c r="J56" s="20"/>
     </row>
-    <row r="57" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>191</v>
       </c>
@@ -2594,7 +2595,7 @@
       <c r="I57" s="5"/>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>129</v>
       </c>
@@ -2607,11 +2608,11 @@
       <c r="I58" s="5"/>
       <c r="J58" s="6"/>
     </row>
-    <row r="59" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I59" s="5"/>
       <c r="J59" s="6"/>
     </row>
-    <row r="60" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C60" s="36" t="s">
         <v>84</v>
       </c>
@@ -2620,7 +2621,7 @@
       <c r="I60" s="5"/>
       <c r="J60" s="6"/>
     </row>
-    <row r="61" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C61" s="7" t="s">
         <v>38</v>
       </c>
@@ -2666,7 +2667,7 @@
       </c>
       <c r="J62" s="20"/>
     </row>
-    <row r="63" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>157</v>
       </c>
@@ -2714,7 +2715,7 @@
       </c>
       <c r="J64" s="20"/>
     </row>
-    <row r="65" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>158</v>
       </c>
@@ -2766,7 +2767,7 @@
       </c>
       <c r="J66" s="20"/>
     </row>
-    <row r="67" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>159</v>
       </c>
@@ -2814,7 +2815,7 @@
       </c>
       <c r="J68" s="20"/>
     </row>
-    <row r="69" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>160</v>
       </c>
@@ -2862,7 +2863,7 @@
       </c>
       <c r="J70" s="20"/>
     </row>
-    <row r="71" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>161</v>
       </c>
@@ -2908,7 +2909,7 @@
       </c>
       <c r="J72" s="20"/>
     </row>
-    <row r="73" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>164</v>
       </c>
@@ -2960,7 +2961,7 @@
       </c>
       <c r="J74" s="20"/>
     </row>
-    <row r="75" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>165</v>
       </c>
@@ -3012,7 +3013,7 @@
       </c>
       <c r="J76" s="20"/>
     </row>
-    <row r="77" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>166</v>
       </c>
@@ -3062,7 +3063,7 @@
       </c>
       <c r="J78" s="20"/>
     </row>
-    <row r="79" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>167</v>
       </c>
@@ -3114,7 +3115,7 @@
       </c>
       <c r="J80" s="20"/>
     </row>
-    <row r="81" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>171</v>
       </c>
@@ -3166,7 +3167,7 @@
       </c>
       <c r="J82" s="20"/>
     </row>
-    <row r="83" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>172</v>
       </c>
@@ -3218,7 +3219,7 @@
       </c>
       <c r="J84" s="20"/>
     </row>
-    <row r="85" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>173</v>
       </c>
@@ -3240,7 +3241,7 @@
       <c r="I85" s="5"/>
       <c r="J85" s="6"/>
     </row>
-    <row r="86" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="16" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>129</v>
       </c>
@@ -3602,7 +3603,13 @@
       <c r="G157" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="G6:G86" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="G6:G86" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="AHLWWLBBXX"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="C86:E86"/>
     <mergeCell ref="C6:E6"/>

</xml_diff>